<commit_message>
Letzte Änderungen am CircuitProject und der Microcode Tabelle Sind nur kleine Änderungen und ist nicht viel dazugekommen. Nur ein wenig Herumgeklicke.
</commit_message>
<xml_diff>
--- a/Microcode.xlsx
+++ b/Microcode.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Reset</t>
   </si>
@@ -55,6 +55,24 @@
   </si>
   <si>
     <t>PC + 1 -&gt; PC</t>
+  </si>
+  <si>
+    <t>C=1 : A -&gt; PC</t>
+  </si>
+  <si>
+    <t>Z=1 : A -&gt; PC</t>
+  </si>
+  <si>
+    <t>Z=0 : PC + 1 -&gt; PC</t>
+  </si>
+  <si>
+    <t>C=0 : PC + 1 -&gt; PC</t>
+  </si>
+  <si>
+    <t>MCU D -&gt; A</t>
+  </si>
+  <si>
+    <t>A -&gt; MCU D</t>
   </si>
 </sst>
 </file>
@@ -389,20 +407,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:Q1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="11" width="11.42578125" style="1"/>
     <col min="12" max="12" width="18.140625" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="11.42578125" style="1"/>
+    <col min="14" max="14" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:23">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -437,7 +463,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:23">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -474,8 +500,38 @@
       <c r="M2" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="N2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:23">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -516,7 +572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:23">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -559,6 +615,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>